<commit_message>
Revert "Merge remote-tracking branch 'origin/master'"
This reverts commit 7b5e5793e3397d3423e99c29cee9024c7e44026f.
</commit_message>
<xml_diff>
--- a/GameJam9/GameJam9/Content/Maptest2.xlsx
+++ b/GameJam9/GameJam9/Content/Maptest2.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="9756" windowHeight="7320"/>
   </bookViews>
   <sheets>
-    <sheet name="Maptest2" sheetId="1" r:id="rId1"/>
+    <sheet name="Maptest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,42 +24,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="11">
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>fg</t>
-  </si>
-  <si>
-    <t>iK</t>
-  </si>
-  <si>
-    <t>E4</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>P</t>
-  </si>
-  <si>
-    <t>fg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>fg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E4</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -456,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC18" sqref="AC18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AU14" sqref="AU14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.09765625" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -2582,7 +2553,7 @@
       <c r="U9">
         <v>0</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9">
         <v>0</v>
       </c>
       <c r="W9">
@@ -2615,8 +2586,8 @@
       <c r="AF9">
         <v>0</v>
       </c>
-      <c r="AG9" t="s">
-        <v>9</v>
+      <c r="AG9">
+        <v>0</v>
       </c>
       <c r="AH9">
         <v>0</v>
@@ -2866,14 +2837,14 @@
       <c r="AD10">
         <v>0</v>
       </c>
-      <c r="AE10" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>1</v>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
       </c>
       <c r="AG10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH10">
         <v>0</v>
@@ -2884,8 +2855,8 @@
       <c r="AJ10">
         <v>0</v>
       </c>
-      <c r="AK10" t="s">
-        <v>8</v>
+      <c r="AK10">
+        <v>0</v>
       </c>
       <c r="AL10">
         <v>0</v>
@@ -2896,17 +2867,17 @@
       <c r="AN10">
         <v>0</v>
       </c>
-      <c r="AO10" t="s">
-        <v>1</v>
+      <c r="AO10">
+        <v>0</v>
       </c>
       <c r="AP10">
         <v>0</v>
       </c>
-      <c r="AQ10" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>1</v>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
       </c>
       <c r="AS10">
         <v>0</v>
@@ -3124,13 +3095,13 @@
         <v>0</v>
       </c>
       <c r="AE11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH11">
         <v>0</v>
@@ -3154,16 +3125,16 @@
         <v>0</v>
       </c>
       <c r="AO11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AP11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AQ11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AR11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AS11">
         <v>0</v>
@@ -3341,14 +3312,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12" t="s">
-        <v>1</v>
+      <c r="R12">
+        <v>0</v>
       </c>
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12" t="s">
-        <v>1</v>
+      <c r="T12">
+        <v>0</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -3362,11 +3333,11 @@
       <c r="X12">
         <v>0</v>
       </c>
-      <c r="Y12" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>1</v>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
       </c>
       <c r="AA12">
         <v>0</v>
@@ -3384,10 +3355,10 @@
         <v>0</v>
       </c>
       <c r="AF12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH12">
         <v>0</v>
@@ -3414,13 +3385,13 @@
         <v>0</v>
       </c>
       <c r="AP12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS12">
         <v>0</v>
@@ -3434,11 +3405,11 @@
       <c r="AV12">
         <v>0</v>
       </c>
-      <c r="AW12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>1</v>
+      <c r="AW12">
+        <v>0</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
       </c>
       <c r="AY12">
         <v>0</v>
@@ -3476,7 +3447,7 @@
       <c r="BJ12">
         <v>0</v>
       </c>
-      <c r="BK12" t="s">
+      <c r="BK12">
         <v>0</v>
       </c>
       <c r="BL12">
@@ -3596,19 +3567,19 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V13">
         <v>0</v>
@@ -3616,15 +3587,15 @@
       <c r="W13">
         <v>0</v>
       </c>
-      <c r="X13" t="s">
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
         <v>1</v>
       </c>
-      <c r="Y13">
-        <v>3</v>
-      </c>
-      <c r="Z13">
-        <v>3</v>
-      </c>
       <c r="AA13">
         <v>0</v>
       </c>
@@ -3643,8 +3614,8 @@
       <c r="AF13">
         <v>0</v>
       </c>
-      <c r="AG13">
-        <v>0</v>
+      <c r="AG13" t="s">
+        <v>1</v>
       </c>
       <c r="AH13">
         <v>0</v>
@@ -3670,14 +3641,14 @@
       <c r="AO13">
         <v>0</v>
       </c>
-      <c r="AP13">
-        <v>0</v>
+      <c r="AP13" t="s">
+        <v>1</v>
       </c>
       <c r="AQ13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -3689,13 +3660,13 @@
         <v>0</v>
       </c>
       <c r="AV13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AW13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AX13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AY13">
         <v>0</v>
@@ -3784,14 +3755,14 @@
       <c r="CA13">
         <v>0</v>
       </c>
-      <c r="CB13" t="s">
-        <v>1</v>
+      <c r="CB13">
+        <v>0</v>
       </c>
       <c r="CC13">
-        <v>3</v>
-      </c>
-      <c r="CD13" t="s">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="CD13">
+        <v>0</v>
       </c>
       <c r="CE13">
         <v>0</v>
@@ -3805,13 +3776,13 @@
     </row>
     <row r="14" spans="1:85" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3832,37 +3803,37 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O14" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -3871,19 +3842,19 @@
         <v>0</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X14">
         <v>3</v>
       </c>
       <c r="Y14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB14">
         <v>0</v>
@@ -3891,8 +3862,8 @@
       <c r="AC14">
         <v>0</v>
       </c>
-      <c r="AD14">
-        <v>0</v>
+      <c r="AD14" t="s">
+        <v>1</v>
       </c>
       <c r="AE14">
         <v>0</v>
@@ -3901,22 +3872,22 @@
         <v>0</v>
       </c>
       <c r="AG14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI14">
         <v>0</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" t="s">
         <v>0</v>
       </c>
       <c r="AK14">
         <v>0</v>
       </c>
-      <c r="AL14">
-        <v>0</v>
+      <c r="AL14" t="s">
+        <v>1</v>
       </c>
       <c r="AM14">
         <v>0</v>
@@ -3928,10 +3899,10 @@
         <v>0</v>
       </c>
       <c r="AP14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR14">
         <v>0</v>
@@ -3949,31 +3920,31 @@
         <v>0</v>
       </c>
       <c r="AW14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AX14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AY14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AZ14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BB14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BC14">
         <v>0</v>
       </c>
-      <c r="BD14" t="s">
-        <v>1</v>
-      </c>
-      <c r="BE14" t="s">
-        <v>1</v>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>0</v>
       </c>
       <c r="BF14">
         <v>0</v>
@@ -3985,58 +3956,58 @@
         <v>0</v>
       </c>
       <c r="BI14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BJ14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BK14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BL14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BM14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BN14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BO14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BP14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BQ14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BR14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BS14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BT14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BU14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BV14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BW14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BX14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BY14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BZ14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CA14">
         <v>3</v>
@@ -4045,255 +4016,255 @@
         <v>3</v>
       </c>
       <c r="CC14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CD14">
         <v>3</v>
       </c>
-      <c r="CE14" t="s">
-        <v>1</v>
+      <c r="CE14">
+        <v>3</v>
       </c>
       <c r="CF14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CG14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:85" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
         <v>3</v>
       </c>
-      <c r="O15">
+      <c r="W15">
+        <v>2</v>
+      </c>
+      <c r="X15">
+        <v>2</v>
+      </c>
+      <c r="Y15">
+        <v>2</v>
+      </c>
+      <c r="Z15">
+        <v>2</v>
+      </c>
+      <c r="AA15">
+        <v>2</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>1</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
         <v>3</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>2</v>
-      </c>
-      <c r="S15">
-        <v>2</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
-        <v>0</v>
-      </c>
-      <c r="X15">
-        <v>2</v>
-      </c>
-      <c r="Y15">
-        <v>2</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>0</v>
-      </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
       <c r="AG15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BB15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BC15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BD15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BE15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BF15">
-        <v>3</v>
-      </c>
-      <c r="BG15" t="s">
         <v>1</v>
       </c>
+      <c r="BG15">
+        <v>1</v>
+      </c>
       <c r="BH15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BJ15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BK15">
-        <v>0</v>
-      </c>
-      <c r="BL15" t="s">
-        <v>1</v>
-      </c>
-      <c r="BM15" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BL15">
+        <v>2</v>
+      </c>
+      <c r="BM15">
+        <v>2</v>
       </c>
       <c r="BN15">
-        <v>0</v>
-      </c>
-      <c r="BO15" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BO15">
+        <v>2</v>
       </c>
       <c r="BP15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BQ15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BR15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BT15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BU15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BV15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BW15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BX15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BY15">
-        <v>0</v>
-      </c>
-      <c r="BZ15" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BZ15">
+        <v>2</v>
       </c>
       <c r="CA15">
         <v>2</v>
@@ -4308,54 +4279,54 @@
         <v>2</v>
       </c>
       <c r="CE15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CF15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CG15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:85" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
       </c>
       <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
       </c>
       <c r="M16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -4363,29 +4334,29 @@
       <c r="O16">
         <v>2</v>
       </c>
-      <c r="P16" t="s">
-        <v>1</v>
+      <c r="P16">
+        <v>2</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
       </c>
       <c r="X16">
         <v>2</v>
@@ -4393,92 +4364,92 @@
       <c r="Y16">
         <v>2</v>
       </c>
-      <c r="Z16" t="s">
-        <v>1</v>
+      <c r="Z16">
+        <v>2</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF16">
-        <v>0</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AG16">
+        <v>2</v>
       </c>
       <c r="AH16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO16">
-        <v>0</v>
-      </c>
-      <c r="AP16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AP16">
+        <v>2</v>
       </c>
       <c r="AQ16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AS16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AV16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AX16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AY16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ16">
-        <v>0</v>
-      </c>
-      <c r="BA16" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BA16">
+        <v>2</v>
+      </c>
+      <c r="BB16">
+        <v>2</v>
       </c>
       <c r="BC16">
         <v>2</v>
@@ -4493,64 +4464,64 @@
         <v>2</v>
       </c>
       <c r="BG16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BH16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BI16">
-        <v>0</v>
-      </c>
-      <c r="BJ16" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="BJ16">
+        <v>2</v>
       </c>
       <c r="BK16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BL16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BM16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BN16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BO16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BP16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BQ16">
-        <v>0</v>
-      </c>
-      <c r="BR16" t="s">
-        <v>4</v>
-      </c>
-      <c r="BS16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BR16">
+        <v>2</v>
+      </c>
+      <c r="BS16">
+        <v>2</v>
       </c>
       <c r="BT16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BU16">
-        <v>0</v>
-      </c>
-      <c r="BV16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BV16">
+        <v>2</v>
       </c>
       <c r="BW16">
-        <v>0</v>
-      </c>
-      <c r="BX16" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BX16">
+        <v>2</v>
       </c>
       <c r="BY16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BZ16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CA16">
         <v>2</v>
@@ -4567,49 +4538,49 @@
       <c r="CE16">
         <v>2</v>
       </c>
-      <c r="CF16" t="s">
-        <v>1</v>
+      <c r="CF16">
+        <v>2</v>
       </c>
       <c r="CG16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:85" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>2</v>
@@ -4621,28 +4592,28 @@
         <v>2</v>
       </c>
       <c r="P17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
-        <v>3</v>
-      </c>
-      <c r="U17" t="s">
-        <v>1</v>
-      </c>
-      <c r="V17" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <v>2</v>
       </c>
       <c r="W17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X17">
         <v>2</v>
@@ -4651,91 +4622,91 @@
         <v>2</v>
       </c>
       <c r="Z17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB17">
-        <v>0</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>2</v>
+      </c>
+      <c r="AD17">
+        <v>2</v>
       </c>
       <c r="AE17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH17">
-        <v>3</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="AI17">
+        <v>2</v>
+      </c>
+      <c r="AJ17">
+        <v>2</v>
       </c>
       <c r="AK17">
-        <v>0</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="AL17">
+        <v>2</v>
+      </c>
+      <c r="AM17">
+        <v>2</v>
       </c>
       <c r="AN17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ17">
-        <v>3</v>
-      </c>
-      <c r="AR17" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AR17">
+        <v>2</v>
       </c>
       <c r="AS17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT17">
-        <v>0</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AU17">
+        <v>2</v>
+      </c>
+      <c r="AV17">
+        <v>2</v>
       </c>
       <c r="AW17">
-        <v>0</v>
-      </c>
-      <c r="AX17" t="s">
-        <v>3</v>
-      </c>
-      <c r="AY17" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AX17">
+        <v>2</v>
+      </c>
+      <c r="AY17">
+        <v>2</v>
       </c>
       <c r="AZ17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BA17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BB17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BC17">
         <v>2</v>
@@ -4756,13 +4727,13 @@
         <v>2</v>
       </c>
       <c r="BI17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BJ17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BK17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BL17">
         <v>2</v>
@@ -4777,34 +4748,34 @@
         <v>2</v>
       </c>
       <c r="BP17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BQ17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BR17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BS17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BT17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BU17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BV17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BW17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BX17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BY17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BZ17">
         <v>2</v>
@@ -4825,10 +4796,10 @@
         <v>2</v>
       </c>
       <c r="CF17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="CG17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:85" x14ac:dyDescent="0.45">
@@ -4839,25 +4810,25 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18">
         <v>2</v>
@@ -4881,22 +4852,22 @@
         <v>2</v>
       </c>
       <c r="Q18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W18">
         <v>2</v>
@@ -4914,19 +4885,19 @@
         <v>2</v>
       </c>
       <c r="AB18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG18">
         <v>2</v>
@@ -4935,25 +4906,25 @@
         <v>2</v>
       </c>
       <c r="AI18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AJ18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AM18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AP18">
         <v>2</v>
@@ -4962,28 +4933,28 @@
         <v>2</v>
       </c>
       <c r="AR18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AS18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AU18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AV18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AY18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ18">
         <v>2</v>

</xml_diff>